<commit_message>
[ER-common] format code, change file name
</commit_message>
<xml_diff>
--- a/3.Js/vue/er-system/checklists/checklist_code_OMProject_DuyNH.xlsx
+++ b/3.Js/vue/er-system/checklists/checklist_code_OMProject_DuyNH.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\TRAININGGG\training_web\3.Js\vue\er-system\checklists\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -168,7 +168,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="90">
   <si>
     <t>Code Review Checklist</t>
   </si>
@@ -249,9 +249,6 @@
   </si>
   <si>
     <t>Mỗi dòng code (kể cả HTML) tối đa 120 ký tự?</t>
-  </si>
-  <si>
-    <t>Các function cách nhau bằng một dòng trống?</t>
   </si>
   <si>
     <t xml:space="preserve">Các function và code phức tạp có comment tiếng Anh? </t>
@@ -544,10 +541,10 @@
     <t>o</t>
   </si>
   <si>
-    <t>Comment ở đầu func</t>
+    <t>space: 2</t>
   </si>
   <si>
-    <t>space: 2</t>
+    <t>Comment ở đầu function</t>
   </si>
 </sst>
 </file>
@@ -1540,8 +1537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1926,7 +1923,7 @@
         <v>15</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
@@ -1958,7 +1955,7 @@
         <v>16</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="15"/>
@@ -1989,7 +1986,7 @@
         <v>17</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
@@ -2051,7 +2048,7 @@
         <v>19</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
@@ -2083,7 +2080,7 @@
         <v>20</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
@@ -2116,7 +2113,7 @@
       </c>
       <c r="B19" s="15"/>
       <c r="C19" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
@@ -2147,7 +2144,7 @@
         <v>22</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="15"/>
@@ -2179,7 +2176,7 @@
         <v>23</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C21" s="15"/>
       <c r="D21" s="15"/>
@@ -2241,13 +2238,13 @@
         <v>25</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C23" s="18"/>
       <c r="D23" s="18"/>
       <c r="E23" s="15"/>
       <c r="F23" s="16" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
@@ -2275,7 +2272,7 @@
         <v>26</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C24" s="18"/>
       <c r="D24" s="18"/>
@@ -2303,11 +2300,11 @@
       <c r="Z24" s="4"/>
     </row>
     <row r="25" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="21" t="s">
-        <v>27</v>
+      <c r="A25" s="20" t="s">
+        <v>26</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C25" s="15"/>
       <c r="D25" s="15"/>
@@ -2336,10 +2333,10 @@
     </row>
     <row r="26" spans="1:26" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A26" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C26" s="15"/>
       <c r="D26" s="15"/>
@@ -2370,13 +2367,12 @@
     </row>
     <row r="27" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A27" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
-      <c r="B27" s="22"/>
+      <c r="B27" s="15" t="s">
+        <v>87</v>
+      </c>
       <c r="C27" s="15"/>
-      <c r="D27" s="15" t="s">
-        <v>88</v>
-      </c>
       <c r="E27" s="15"/>
       <c r="F27" s="16"/>
       <c r="G27" s="4"/>
@@ -2402,10 +2398,10 @@
     </row>
     <row r="28" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A28" s="21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C28" s="15"/>
       <c r="D28" s="15"/>
@@ -2434,11 +2430,10 @@
     </row>
     <row r="29" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A29" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
-      <c r="B29" s="22"/>
-      <c r="C29" s="15" t="s">
-        <v>88</v>
+      <c r="B29" s="15" t="s">
+        <v>87</v>
       </c>
       <c r="D29" s="15"/>
       <c r="E29" s="15"/>
@@ -2466,11 +2461,11 @@
     </row>
     <row r="30" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A30" s="21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B30" s="22"/>
       <c r="C30" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D30" s="15"/>
       <c r="E30" s="15"/>
@@ -2498,11 +2493,11 @@
     </row>
     <row r="31" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A31" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B31" s="22"/>
       <c r="C31" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D31" s="15"/>
       <c r="E31" s="15"/>
@@ -2530,10 +2525,10 @@
     </row>
     <row r="32" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A32" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C32" s="15"/>
       <c r="D32" s="15"/>
@@ -2562,7 +2557,7 @@
     </row>
     <row r="33" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B33" s="43"/>
       <c r="C33" s="43"/>
@@ -2592,10 +2587,10 @@
     </row>
     <row r="34" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A34" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C34" s="22"/>
       <c r="D34" s="22"/>
@@ -2624,10 +2619,10 @@
     </row>
     <row r="35" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A35" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B35" s="22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C35" s="15"/>
       <c r="D35" s="15"/>
@@ -2656,11 +2651,11 @@
     </row>
     <row r="36" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A36" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B36" s="22"/>
       <c r="C36" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D36" s="15"/>
       <c r="E36" s="15"/>
@@ -2688,10 +2683,10 @@
     </row>
     <row r="37" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A37" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B37" s="22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C37" s="15"/>
       <c r="D37" s="15"/>
@@ -2720,10 +2715,10 @@
     </row>
     <row r="38" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A38" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B38" s="22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C38" s="15"/>
       <c r="D38" s="15"/>
@@ -2752,11 +2747,11 @@
     </row>
     <row r="39" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A39" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B39" s="22"/>
       <c r="C39" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D39" s="15"/>
       <c r="E39" s="15"/>
@@ -2784,10 +2779,10 @@
     </row>
     <row r="40" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A40" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B40" s="22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C40" s="15"/>
       <c r="D40" s="15"/>
@@ -2816,10 +2811,10 @@
     </row>
     <row r="41" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A41" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C41" s="15"/>
       <c r="D41" s="15"/>
@@ -2848,7 +2843,7 @@
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B42" s="43"/>
       <c r="C42" s="43"/>
@@ -2878,11 +2873,11 @@
     </row>
     <row r="43" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A43" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B43" s="15"/>
       <c r="C43" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D43" s="15"/>
       <c r="E43" s="15"/>
@@ -2910,10 +2905,10 @@
     </row>
     <row r="44" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A44" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B44" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C44" s="15"/>
       <c r="D44" s="15"/>
@@ -2942,10 +2937,10 @@
     </row>
     <row r="45" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A45" s="23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C45" s="15"/>
       <c r="D45" s="15"/>
@@ -2974,10 +2969,10 @@
     </row>
     <row r="46" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A46" s="23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B46" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C46" s="15"/>
       <c r="D46" s="15"/>
@@ -3006,10 +3001,10 @@
     </row>
     <row r="47" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A47" s="23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C47" s="15"/>
       <c r="D47" s="15"/>
@@ -3038,10 +3033,10 @@
     </row>
     <row r="48" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A48" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B48" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C48" s="15"/>
       <c r="D48" s="15"/>
@@ -3070,10 +3065,10 @@
     </row>
     <row r="49" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A49" s="23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B49" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C49" s="15"/>
       <c r="D49" s="15"/>
@@ -3102,11 +3097,10 @@
     </row>
     <row r="50" spans="1:26" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A50" s="24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
-      <c r="B50" s="15"/>
-      <c r="C50" s="15" t="s">
-        <v>88</v>
+      <c r="B50" s="15" t="s">
+        <v>87</v>
       </c>
       <c r="D50" s="15"/>
       <c r="E50" s="15"/>
@@ -3134,11 +3128,11 @@
     </row>
     <row r="51" spans="1:26" ht="44.25" x14ac:dyDescent="0.3">
       <c r="A51" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B51" s="15"/>
       <c r="C51" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D51" s="15"/>
       <c r="E51" s="15"/>
@@ -3166,10 +3160,10 @@
     </row>
     <row r="52" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A52" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B52" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C52" s="15"/>
       <c r="D52" s="15"/>
@@ -3198,10 +3192,10 @@
     </row>
     <row r="53" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A53" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C53" s="15"/>
       <c r="D53" s="15"/>
@@ -3230,10 +3224,10 @@
     </row>
     <row r="54" spans="1:26" ht="131.25" x14ac:dyDescent="0.3">
       <c r="A54" s="26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B54" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C54" s="15"/>
       <c r="D54" s="15"/>
@@ -3290,7 +3284,7 @@
     </row>
     <row r="56" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B56" s="31"/>
       <c r="C56" s="31"/>
@@ -3320,7 +3314,7 @@
     </row>
     <row r="57" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B57" s="34"/>
       <c r="C57" s="34"/>
@@ -3350,7 +3344,7 @@
     </row>
     <row r="58" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B58" s="34"/>
       <c r="C58" s="34"/>
@@ -3380,7 +3374,7 @@
     </row>
     <row r="59" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B59" s="34"/>
       <c r="C59" s="34"/>
@@ -29813,7 +29807,7 @@
     <row r="2" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A2" s="37"/>
       <c r="B2" s="38" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C2" s="37"/>
       <c r="D2" s="37"/>
@@ -29899,7 +29893,7 @@
     <row r="5" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="36"/>
       <c r="B5" s="39" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C5" s="36"/>
       <c r="D5" s="36"/>
@@ -29957,7 +29951,7 @@
     <row r="7" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="36"/>
       <c r="B7" s="40" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C7" s="36"/>
       <c r="D7" s="36"/>
@@ -30015,7 +30009,7 @@
     <row r="9" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="36"/>
       <c r="B9" s="36" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C9" s="36"/>
       <c r="D9" s="36"/>
@@ -30045,7 +30039,7 @@
     <row r="10" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="36"/>
       <c r="B10" s="41" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C10" s="36"/>
       <c r="D10" s="36"/>
@@ -30131,7 +30125,7 @@
     <row r="13" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="36"/>
       <c r="B13" s="40" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C13" s="36"/>
       <c r="D13" s="36"/>
@@ -30161,7 +30155,7 @@
     <row r="14" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="36"/>
       <c r="B14" s="36" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C14" s="36"/>
       <c r="D14" s="36"/>
@@ -30667,7 +30661,7 @@
     <row r="32" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="36"/>
       <c r="B32" s="40" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C32" s="36"/>
       <c r="D32" s="36"/>
@@ -30697,7 +30691,7 @@
     <row r="33" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="36"/>
       <c r="B33" s="36" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C33" s="36"/>
       <c r="D33" s="36"/>
@@ -30727,7 +30721,7 @@
     <row r="34" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="36"/>
       <c r="B34" s="36" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C34" s="36"/>
       <c r="D34" s="36"/>
@@ -31149,7 +31143,7 @@
     <row r="49" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="36"/>
       <c r="B49" s="40" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C49" s="36"/>
       <c r="D49" s="36"/>
@@ -31179,7 +31173,7 @@
     <row r="50" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="36"/>
       <c r="B50" s="41" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C50" s="36"/>
       <c r="D50" s="36"/>
@@ -31545,7 +31539,7 @@
     <row r="63" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="36"/>
       <c r="B63" s="40" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C63" s="36"/>
       <c r="D63" s="36"/>
@@ -31575,7 +31569,7 @@
     <row r="64" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="36"/>
       <c r="B64" s="41" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C64" s="36"/>
       <c r="D64" s="36"/>
@@ -31969,7 +31963,7 @@
     <row r="78" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A78" s="36"/>
       <c r="B78" s="39" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C78" s="36"/>
       <c r="D78" s="36"/>
@@ -32755,7 +32749,7 @@
     <row r="106" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A106" s="36"/>
       <c r="B106" s="39" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C106" s="36"/>
       <c r="D106" s="36"/>
@@ -32785,7 +32779,7 @@
     <row r="107" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="36"/>
       <c r="B107" s="41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C107" s="36"/>
       <c r="D107" s="36"/>
@@ -33291,7 +33285,7 @@
     <row r="125" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A125" s="36"/>
       <c r="B125" s="39" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C125" s="36"/>
       <c r="D125" s="36"/>
@@ -33321,7 +33315,7 @@
     <row r="126" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="36"/>
       <c r="B126" s="41" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C126" s="36"/>
       <c r="D126" s="36"/>
@@ -33855,7 +33849,7 @@
     <row r="145" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="36"/>
       <c r="B145" s="41" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C145" s="36"/>
       <c r="D145" s="36"/>
@@ -34165,7 +34159,7 @@
     <row r="156" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A156" s="36"/>
       <c r="B156" s="39" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C156" s="36"/>
       <c r="D156" s="36"/>
@@ -34195,7 +34189,7 @@
     <row r="157" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" s="36"/>
       <c r="B157" s="41" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C157" s="36"/>
       <c r="D157" s="36"/>
@@ -34729,7 +34723,7 @@
     <row r="176" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A176" s="36"/>
       <c r="B176" s="39" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C176" s="36"/>
       <c r="D176" s="36"/>
@@ -34759,7 +34753,7 @@
     <row r="177" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A177" s="36"/>
       <c r="B177" s="41" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C177" s="36"/>
       <c r="D177" s="36"/>
@@ -34789,7 +34783,7 @@
     <row r="178" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A178" s="36"/>
       <c r="B178" s="41" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C178" s="36"/>
       <c r="D178" s="36"/>
@@ -34819,7 +34813,7 @@
     <row r="179" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A179" s="36"/>
       <c r="B179" s="41" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C179" s="36"/>
       <c r="D179" s="36"/>
@@ -34849,7 +34843,7 @@
     <row r="180" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A180" s="36"/>
       <c r="B180" s="41" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C180" s="36"/>
       <c r="D180" s="36"/>

</xml_diff>